<commit_message>
adding new endpoint /grades
</commit_message>
<xml_diff>
--- a/info/data.xlsx
+++ b/info/data.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\miche\web0_practices\employeesAPI\info\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5795C28E-084B-443C-84BD-F99139BFEBFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F37D8D45-A364-477B-97E1-A3F7DC08F881}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="employees" sheetId="1" r:id="rId1"/>
+    <sheet name="grades" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="25">
   <si>
     <t>ID</t>
   </si>
@@ -70,6 +71,36 @@
   </si>
   <si>
     <t>Murielle</t>
+  </si>
+  <si>
+    <t>Course</t>
+  </si>
+  <si>
+    <t>Grade</t>
+  </si>
+  <si>
+    <t>CSCI200</t>
+  </si>
+  <si>
+    <t>Andy</t>
+  </si>
+  <si>
+    <t>Jennifer</t>
+  </si>
+  <si>
+    <t>Maro</t>
+  </si>
+  <si>
+    <t>Gaby</t>
+  </si>
+  <si>
+    <t>Jhon</t>
+  </si>
+  <si>
+    <t>Mary</t>
+  </si>
+  <si>
+    <t>Christy</t>
   </si>
 </sst>
 </file>
@@ -422,7 +453,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
@@ -517,4 +548,160 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4A0FA0F-48E0-4524-B723-11814E11D678}">
+  <dimension ref="A1:D10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="2">
+        <v>62210082</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="2">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="2">
+        <v>62201458</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="2">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="2">
+        <v>62204587</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="2">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="2">
+        <v>62204588</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="2">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="2">
+        <v>62204589</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" s="2">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="2">
+        <v>62214587</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="2">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="2">
+        <v>62214487</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" s="2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="2">
+        <v>62214547</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" s="2">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="2">
+        <v>62213587</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" s="2">
+        <v>34</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>